<commit_message>
minor changes to mary'e version of interest, relationship schema on Deirdre file
</commit_message>
<xml_diff>
--- a/Database Implementation/Test Data Generator - Deirdre.xlsx
+++ b/Database Implementation/Test Data Generator - Deirdre.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\501834813\Documents\GitHub\WebProject\Database Implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\WebProject\Database Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="user_profile" sheetId="1" r:id="rId1"/>
+    <sheet name="relationship_type" sheetId="2" r:id="rId2"/>
+    <sheet name="user_interests" sheetId="3" r:id="rId3"/>
+    <sheet name="interests" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">user_profile!$A$1:$L$52</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="112">
   <si>
     <t>password_hash</t>
   </si>
@@ -328,12 +331,42 @@
   </si>
   <si>
     <t>https://homepage.net/name_generator/</t>
+  </si>
+  <si>
+    <t>User_id</t>
+  </si>
+  <si>
+    <t>relationship_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>casual</t>
+  </si>
+  <si>
+    <t>friendship</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>interest_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1218,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1271,7 @@
     <col min="12" max="12" width="162" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1272,12 +1305,9 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="str">
-        <f>"insert into user_profile ("&amp;$A$1&amp;","&amp;$B$1&amp;","&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;","&amp;$F$1&amp;","&amp;$G$1&amp;","&amp;$H$1&amp;","&amp;$I$1&amp;","&amp;$K$1&amp;") values  ('"&amp;A1&amp;"','"&amp;B1&amp;"','"&amp;C1&amp;"','"&amp;D1&amp;"','"&amp;E1&amp;"','"&amp;F1&amp;"','"&amp;G1&amp;"','"&amp;H1&amp;"','"&amp;I1&amp;"','"&amp;K1&amp;"');"</f>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('password_hash','first_name','sur_name','email','date_of_birth','sex','gender_preference','black_listed_user','black_listed_reason','user_status');</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1301,10 +1331,6 @@
       </c>
       <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="L2" s="3" t="str">
-        <f>"insert into user_profile ("&amp;$A$1&amp;","&amp;$B$1&amp;","&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;","&amp;$F$1&amp;","&amp;$G$1&amp;","&amp;$H$1&amp;","&amp;$I$1&amp;","&amp;$K$1&amp;") values  ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;K2&amp;"');"</f>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','John','Doe','john.doe@gmail.com','2000-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2870,4 +2896,140 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>